<commit_message>
Cambios en vista de facturas en AdministerBills, cambios en cerrar, modificar y aplazar facturas para que tomara en cuenta el id de proveedor y que establezca el estado en cerrado, y cree un metodo aparte para aplazar
</commit_message>
<xml_diff>
--- a/UI/Plantilla Proveedores Fact Elec.xlsx
+++ b/UI/Plantilla Proveedores Fact Elec.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\Estudiante\Desktop\Proyecto Transtecno\Proyecto Análisis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF52507-8220-4209-B570-E262B248CFA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="525" windowWidth="15015" windowHeight="7365"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ListaDocAceptacion" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1559" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545" uniqueCount="412">
   <si>
     <t>IdEmpresa</t>
   </si>
@@ -756,12 +762,6 @@
   </si>
   <si>
     <t>00100002030000003721</t>
-  </si>
-  <si>
-    <t>00100001050000001537</t>
-  </si>
-  <si>
-    <t>22600010010000002601</t>
   </si>
   <si>
     <t>3102007223</t>
@@ -1262,10 +1262,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_(&quot;₡&quot;* #,##0.00_);_(&quot;₡&quot;* \(#,##0.00\);_(&quot;₡&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="[$$-540A]#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;₡&quot;* #,##0.00_);_(&quot;₡&quot;* \(#,##0.00\);_(&quot;₡&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="[$$-540A]#,##0.00"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -1296,12 +1296,13 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1309,37 +1310,45 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:X119">
-  <autoFilter ref="A1:X119"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:X118">
+  <autoFilter ref="A1:X118" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="24">
-    <tableColumn id="1" name="IdEmpresa"/>
-    <tableColumn id="2" name="TipoDocRecibido"/>
-    <tableColumn id="3" name="ConsecutivoAceptacion"/>
-    <tableColumn id="4" name="FechaEmisionAceptacion"/>
-    <tableColumn id="5" name="ConsecutivoDocumento"/>
-    <tableColumn id="6" name="TipoDocAceptacion"/>
-    <tableColumn id="7" name="IdentificacionReceptor"/>
-    <tableColumn id="8" name="NombreReceptor"/>
-    <tableColumn id="9" name="ActividadEconomicaReceptor"/>
-    <tableColumn id="10" name="IdentificacionEmisor"/>
-    <tableColumn id="11" name="NombreEmisor"/>
-    <tableColumn id="12" name="ActividadEconomicaEmisor"/>
-    <tableColumn id="13" name="DetalleAceptacion"/>
-    <tableColumn id="14" name="FechaEmisionDocumento"/>
-    <tableColumn id="15" name="EstadoHacienda"/>
-    <tableColumn id="16" name="MensajeHacienda"/>
-    <tableColumn id="17" name="TotalDeGastoAplicable"/>
-    <tableColumn id="18" name="TotalImpuestoAcreditar"/>
-    <tableColumn id="19" name="TotalNeto"/>
-    <tableColumn id="20" name="TotalImpuesto"/>
-    <tableColumn id="21" name="TotalComprobante"/>
-    <tableColumn id="22" name="CodigoMoneda"/>
-    <tableColumn id="23" name="TipoCambio"/>
-    <tableColumn id="24" name="Total Colones"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="IdEmpresa"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="TipoDocRecibido"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="ConsecutivoAceptacion"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="FechaEmisionAceptacion"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="ConsecutivoDocumento"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="TipoDocAceptacion"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="IdentificacionReceptor"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="NombreReceptor"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="ActividadEconomicaReceptor"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="IdentificacionEmisor"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="NombreEmisor"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="ActividadEconomicaEmisor"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="DetalleAceptacion"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="FechaEmisionDocumento"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="EstadoHacienda"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="MensajeHacienda"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="TotalDeGastoAplicable"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="TotalImpuestoAcreditar"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="TotalNeto"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="TotalImpuesto"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="TotalComprobante"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="CodigoMoneda"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="TipoCambio"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Total Colones"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1388,7 +1397,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1420,9 +1429,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1454,6 +1481,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1629,18 +1674,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X119"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K100" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25:U25"/>
+    <sheetView tabSelected="1" topLeftCell="D107" workbookViewId="0">
+      <selection activeCell="N118" sqref="N118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="19" max="19" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -5303,13 +5351,13 @@
         <v>24</v>
       </c>
       <c r="C57" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="D57" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E57" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="F57" t="s">
         <v>28</v>
@@ -5321,16 +5369,16 @@
         <v>30</v>
       </c>
       <c r="J57" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="K57" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="L57" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="N57" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="O57" t="s">
         <v>34</v>
@@ -5342,13 +5390,13 @@
         <v>0</v>
       </c>
       <c r="S57" s="1">
-        <v>124288.82296999999</v>
+        <v>194601.76991</v>
       </c>
       <c r="T57" s="1">
-        <v>9937.1770300000007</v>
+        <v>25298.230090000001</v>
       </c>
       <c r="U57" s="1">
-        <v>134226</v>
+        <v>219900</v>
       </c>
       <c r="V57" t="s">
         <v>35</v>
@@ -5357,7 +5405,7 @@
         <v>1</v>
       </c>
       <c r="X57">
-        <v>134226</v>
+        <v>219900</v>
       </c>
     </row>
     <row r="58" spans="1:24">
@@ -5368,13 +5416,13 @@
         <v>24</v>
       </c>
       <c r="C58" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="D58" t="s">
         <v>66</v>
       </c>
       <c r="E58" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="F58" t="s">
         <v>28</v>
@@ -5386,16 +5434,16 @@
         <v>30</v>
       </c>
       <c r="J58" t="s">
-        <v>254</v>
+        <v>88</v>
       </c>
       <c r="K58" t="s">
-        <v>255</v>
+        <v>89</v>
       </c>
       <c r="L58" t="s">
-        <v>256</v>
+        <v>90</v>
       </c>
       <c r="N58" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
       <c r="O58" t="s">
         <v>34</v>
@@ -5407,13 +5455,13 @@
         <v>0</v>
       </c>
       <c r="S58" s="1">
-        <v>194601.76991</v>
+        <v>30800</v>
       </c>
       <c r="T58" s="1">
-        <v>25298.230090000001</v>
+        <v>4004</v>
       </c>
       <c r="U58" s="1">
-        <v>219900</v>
+        <v>34804</v>
       </c>
       <c r="V58" t="s">
         <v>35</v>
@@ -5422,7 +5470,7 @@
         <v>1</v>
       </c>
       <c r="X58">
-        <v>219900</v>
+        <v>34804</v>
       </c>
     </row>
     <row r="59" spans="1:24">
@@ -5436,7 +5484,7 @@
         <v>257</v>
       </c>
       <c r="D59" t="s">
-        <v>66</v>
+        <v>234</v>
       </c>
       <c r="E59" t="s">
         <v>258</v>
@@ -5451,16 +5499,16 @@
         <v>30</v>
       </c>
       <c r="J59" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="K59" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="L59" t="s">
-        <v>90</v>
+        <v>33</v>
       </c>
       <c r="N59" t="s">
-        <v>101</v>
+        <v>234</v>
       </c>
       <c r="O59" t="s">
         <v>34</v>
@@ -5472,13 +5520,13 @@
         <v>0</v>
       </c>
       <c r="S59" s="1">
-        <v>30800</v>
+        <v>3500</v>
       </c>
       <c r="T59" s="1">
-        <v>4004</v>
+        <v>0</v>
       </c>
       <c r="U59" s="1">
-        <v>34804</v>
+        <v>3500</v>
       </c>
       <c r="V59" t="s">
         <v>35</v>
@@ -5487,7 +5535,7 @@
         <v>1</v>
       </c>
       <c r="X59">
-        <v>34804</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="60" spans="1:24">
@@ -5501,7 +5549,7 @@
         <v>259</v>
       </c>
       <c r="D60" t="s">
-        <v>234</v>
+        <v>37</v>
       </c>
       <c r="E60" t="s">
         <v>260</v>
@@ -5516,16 +5564,16 @@
         <v>30</v>
       </c>
       <c r="J60" t="s">
-        <v>31</v>
+        <v>138</v>
       </c>
       <c r="K60" t="s">
-        <v>32</v>
+        <v>139</v>
       </c>
       <c r="L60" t="s">
-        <v>33</v>
+        <v>140</v>
       </c>
       <c r="N60" t="s">
-        <v>234</v>
+        <v>77</v>
       </c>
       <c r="O60" t="s">
         <v>34</v>
@@ -5537,13 +5585,13 @@
         <v>0</v>
       </c>
       <c r="S60" s="1">
-        <v>3500</v>
+        <v>299285.71000000002</v>
       </c>
       <c r="T60" s="1">
-        <v>0</v>
+        <v>11053.5074</v>
       </c>
       <c r="U60" s="1">
-        <v>3500</v>
+        <v>310339.21740000002</v>
       </c>
       <c r="V60" t="s">
         <v>35</v>
@@ -5552,7 +5600,7 @@
         <v>1</v>
       </c>
       <c r="X60">
-        <v>3500</v>
+        <v>310339.21740000002</v>
       </c>
     </row>
     <row r="61" spans="1:24">
@@ -5566,7 +5614,7 @@
         <v>261</v>
       </c>
       <c r="D61" t="s">
-        <v>37</v>
+        <v>242</v>
       </c>
       <c r="E61" t="s">
         <v>262</v>
@@ -5581,16 +5629,16 @@
         <v>30</v>
       </c>
       <c r="J61" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="K61" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
       <c r="L61" t="s">
-        <v>140</v>
+        <v>155</v>
       </c>
       <c r="N61" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="O61" t="s">
         <v>34</v>
@@ -5602,13 +5650,13 @@
         <v>0</v>
       </c>
       <c r="S61" s="1">
-        <v>299285.71000000002</v>
+        <v>15221.25</v>
       </c>
       <c r="T61" s="1">
-        <v>11053.5074</v>
+        <v>1978.76</v>
       </c>
       <c r="U61" s="1">
-        <v>310339.21740000002</v>
+        <v>17200.009999999998</v>
       </c>
       <c r="V61" t="s">
         <v>35</v>
@@ -5617,7 +5665,7 @@
         <v>1</v>
       </c>
       <c r="X61">
-        <v>310339.21740000002</v>
+        <v>17200.009999999998</v>
       </c>
     </row>
     <row r="62" spans="1:24">
@@ -5631,7 +5679,7 @@
         <v>263</v>
       </c>
       <c r="D62" t="s">
-        <v>242</v>
+        <v>44</v>
       </c>
       <c r="E62" t="s">
         <v>264</v>
@@ -5646,16 +5694,16 @@
         <v>30</v>
       </c>
       <c r="J62" t="s">
-        <v>153</v>
+        <v>62</v>
       </c>
       <c r="K62" t="s">
-        <v>154</v>
+        <v>63</v>
       </c>
       <c r="L62" t="s">
-        <v>155</v>
+        <v>64</v>
       </c>
       <c r="N62" t="s">
-        <v>79</v>
+        <v>265</v>
       </c>
       <c r="O62" t="s">
         <v>34</v>
@@ -5667,13 +5715,13 @@
         <v>0</v>
       </c>
       <c r="S62" s="1">
-        <v>15221.25</v>
+        <v>31081.88</v>
       </c>
       <c r="T62" s="1">
-        <v>1978.76</v>
+        <v>4040.65</v>
       </c>
       <c r="U62" s="1">
-        <v>17200.009999999998</v>
+        <v>35122.53</v>
       </c>
       <c r="V62" t="s">
         <v>35</v>
@@ -5682,7 +5730,7 @@
         <v>1</v>
       </c>
       <c r="X62">
-        <v>17200.009999999998</v>
+        <v>35122.53</v>
       </c>
     </row>
     <row r="63" spans="1:24">
@@ -5693,13 +5741,13 @@
         <v>24</v>
       </c>
       <c r="C63" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D63" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="E63" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F63" t="s">
         <v>28</v>
@@ -5711,16 +5759,16 @@
         <v>30</v>
       </c>
       <c r="J63" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="K63" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="L63" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="N63" t="s">
-        <v>267</v>
+        <v>91</v>
       </c>
       <c r="O63" t="s">
         <v>34</v>
@@ -5732,13 +5780,13 @@
         <v>0</v>
       </c>
       <c r="S63" s="1">
-        <v>31081.88</v>
+        <v>3500</v>
       </c>
       <c r="T63" s="1">
-        <v>4040.65</v>
+        <v>0</v>
       </c>
       <c r="U63" s="1">
-        <v>35122.53</v>
+        <v>3500</v>
       </c>
       <c r="V63" t="s">
         <v>35</v>
@@ -5747,7 +5795,7 @@
         <v>1</v>
       </c>
       <c r="X63">
-        <v>35122.53</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="64" spans="1:24">
@@ -5755,13 +5803,13 @@
         <v>39015</v>
       </c>
       <c r="B64" t="s">
-        <v>24</v>
+        <v>121</v>
       </c>
       <c r="C64" t="s">
         <v>268</v>
       </c>
       <c r="D64" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E64" t="s">
         <v>269</v>
@@ -5776,16 +5824,16 @@
         <v>30</v>
       </c>
       <c r="J64" t="s">
-        <v>31</v>
+        <v>144</v>
       </c>
       <c r="K64" t="s">
-        <v>32</v>
+        <v>145</v>
       </c>
       <c r="L64" t="s">
-        <v>33</v>
+        <v>146</v>
       </c>
       <c r="N64" t="s">
-        <v>91</v>
+        <v>126</v>
       </c>
       <c r="O64" t="s">
         <v>34</v>
@@ -5797,13 +5845,13 @@
         <v>0</v>
       </c>
       <c r="S64" s="1">
-        <v>3500</v>
+        <v>36251.61</v>
       </c>
       <c r="T64" s="1">
-        <v>0</v>
+        <v>4712.71</v>
       </c>
       <c r="U64" s="1">
-        <v>3500</v>
+        <v>40964.32</v>
       </c>
       <c r="V64" t="s">
         <v>35</v>
@@ -5812,7 +5860,7 @@
         <v>1</v>
       </c>
       <c r="X64">
-        <v>3500</v>
+        <v>40964.32</v>
       </c>
     </row>
     <row r="65" spans="1:24">
@@ -5820,13 +5868,13 @@
         <v>39015</v>
       </c>
       <c r="B65" t="s">
-        <v>121</v>
+        <v>24</v>
       </c>
       <c r="C65" t="s">
         <v>270</v>
       </c>
       <c r="D65" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E65" t="s">
         <v>271</v>
@@ -5841,16 +5889,16 @@
         <v>30</v>
       </c>
       <c r="J65" t="s">
-        <v>144</v>
+        <v>31</v>
       </c>
       <c r="K65" t="s">
-        <v>145</v>
+        <v>32</v>
       </c>
       <c r="L65" t="s">
-        <v>146</v>
+        <v>33</v>
       </c>
       <c r="N65" t="s">
-        <v>126</v>
+        <v>71</v>
       </c>
       <c r="O65" t="s">
         <v>34</v>
@@ -5862,13 +5910,13 @@
         <v>0</v>
       </c>
       <c r="S65" s="1">
-        <v>36251.61</v>
+        <v>3500</v>
       </c>
       <c r="T65" s="1">
-        <v>4712.71</v>
+        <v>0</v>
       </c>
       <c r="U65" s="1">
-        <v>40964.32</v>
+        <v>3500</v>
       </c>
       <c r="V65" t="s">
         <v>35</v>
@@ -5877,7 +5925,7 @@
         <v>1</v>
       </c>
       <c r="X65">
-        <v>40964.32</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="66" spans="1:24">
@@ -5906,16 +5954,16 @@
         <v>30</v>
       </c>
       <c r="J66" t="s">
-        <v>31</v>
+        <v>274</v>
       </c>
       <c r="K66" t="s">
-        <v>32</v>
+        <v>275</v>
       </c>
       <c r="L66" t="s">
         <v>33</v>
       </c>
       <c r="N66" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="O66" t="s">
         <v>34</v>
@@ -5927,13 +5975,13 @@
         <v>0</v>
       </c>
       <c r="S66" s="1">
-        <v>3500</v>
+        <v>11806.41</v>
       </c>
       <c r="T66" s="1">
-        <v>0</v>
+        <v>1395.3</v>
       </c>
       <c r="U66" s="1">
-        <v>3500</v>
+        <v>13201.71</v>
       </c>
       <c r="V66" t="s">
         <v>35</v>
@@ -5942,7 +5990,7 @@
         <v>1</v>
       </c>
       <c r="X66">
-        <v>3500</v>
+        <v>13201.71</v>
       </c>
     </row>
     <row r="67" spans="1:24">
@@ -5953,13 +6001,13 @@
         <v>24</v>
       </c>
       <c r="C67" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D67" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="E67" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F67" t="s">
         <v>28</v>
@@ -5971,16 +6019,16 @@
         <v>30</v>
       </c>
       <c r="J67" t="s">
-        <v>276</v>
+        <v>62</v>
       </c>
       <c r="K67" t="s">
-        <v>277</v>
+        <v>63</v>
       </c>
       <c r="L67" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="N67" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="O67" t="s">
         <v>34</v>
@@ -5992,13 +6040,13 @@
         <v>0</v>
       </c>
       <c r="S67" s="1">
-        <v>11806.41</v>
+        <v>10405.76</v>
       </c>
       <c r="T67" s="1">
-        <v>1395.3</v>
+        <v>1352.75</v>
       </c>
       <c r="U67" s="1">
-        <v>13201.71</v>
+        <v>11758.51</v>
       </c>
       <c r="V67" t="s">
         <v>35</v>
@@ -6007,7 +6055,7 @@
         <v>1</v>
       </c>
       <c r="X67">
-        <v>13201.71</v>
+        <v>11758.51</v>
       </c>
     </row>
     <row r="68" spans="1:24">
@@ -6021,7 +6069,7 @@
         <v>278</v>
       </c>
       <c r="D68" t="s">
-        <v>103</v>
+        <v>37</v>
       </c>
       <c r="E68" t="s">
         <v>279</v>
@@ -6036,16 +6084,16 @@
         <v>30</v>
       </c>
       <c r="J68" t="s">
-        <v>62</v>
+        <v>280</v>
       </c>
       <c r="K68" t="s">
-        <v>63</v>
+        <v>281</v>
       </c>
       <c r="L68" t="s">
-        <v>64</v>
+        <v>282</v>
       </c>
       <c r="N68" t="s">
-        <v>103</v>
+        <v>42</v>
       </c>
       <c r="O68" t="s">
         <v>34</v>
@@ -6057,13 +6105,13 @@
         <v>0</v>
       </c>
       <c r="S68" s="1">
-        <v>10405.76</v>
+        <v>35861.35</v>
       </c>
       <c r="T68" s="1">
-        <v>1352.75</v>
+        <v>4661.9754999999996</v>
       </c>
       <c r="U68" s="1">
-        <v>11758.51</v>
+        <v>40523.325499999999</v>
       </c>
       <c r="V68" t="s">
         <v>35</v>
@@ -6072,7 +6120,7 @@
         <v>1</v>
       </c>
       <c r="X68">
-        <v>11758.51</v>
+        <v>40523.325499999999</v>
       </c>
     </row>
     <row r="69" spans="1:24">
@@ -6083,13 +6131,13 @@
         <v>24</v>
       </c>
       <c r="C69" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="D69" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E69" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="F69" t="s">
         <v>28</v>
@@ -6101,16 +6149,16 @@
         <v>30</v>
       </c>
       <c r="J69" t="s">
-        <v>282</v>
+        <v>149</v>
       </c>
       <c r="K69" t="s">
-        <v>283</v>
+        <v>150</v>
       </c>
       <c r="L69" t="s">
-        <v>284</v>
+        <v>64</v>
       </c>
       <c r="N69" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="O69" t="s">
         <v>34</v>
@@ -6122,13 +6170,13 @@
         <v>0</v>
       </c>
       <c r="S69" s="1">
-        <v>35861.35</v>
+        <v>205189.12</v>
       </c>
       <c r="T69" s="1">
-        <v>4661.9754999999996</v>
+        <v>26674.58</v>
       </c>
       <c r="U69" s="1">
-        <v>40523.325499999999</v>
+        <v>231863.7</v>
       </c>
       <c r="V69" t="s">
         <v>35</v>
@@ -6137,7 +6185,7 @@
         <v>1</v>
       </c>
       <c r="X69">
-        <v>40523.325499999999</v>
+        <v>231863.7</v>
       </c>
     </row>
     <row r="70" spans="1:24">
@@ -6151,7 +6199,7 @@
         <v>285</v>
       </c>
       <c r="D70" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E70" t="s">
         <v>286</v>
@@ -6166,16 +6214,16 @@
         <v>30</v>
       </c>
       <c r="J70" t="s">
-        <v>149</v>
+        <v>62</v>
       </c>
       <c r="K70" t="s">
-        <v>150</v>
+        <v>63</v>
       </c>
       <c r="L70" t="s">
         <v>64</v>
       </c>
       <c r="N70" t="s">
-        <v>49</v>
+        <v>117</v>
       </c>
       <c r="O70" t="s">
         <v>34</v>
@@ -6187,13 +6235,13 @@
         <v>0</v>
       </c>
       <c r="S70" s="1">
-        <v>205189.12</v>
+        <v>5322.29</v>
       </c>
       <c r="T70" s="1">
-        <v>26674.58</v>
+        <v>691.9</v>
       </c>
       <c r="U70" s="1">
-        <v>231863.7</v>
+        <v>6014.19</v>
       </c>
       <c r="V70" t="s">
         <v>35</v>
@@ -6202,7 +6250,7 @@
         <v>1</v>
       </c>
       <c r="X70">
-        <v>231863.7</v>
+        <v>6014.19</v>
       </c>
     </row>
     <row r="71" spans="1:24">
@@ -6216,7 +6264,7 @@
         <v>287</v>
       </c>
       <c r="D71" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E71" t="s">
         <v>288</v>
@@ -6231,16 +6279,16 @@
         <v>30</v>
       </c>
       <c r="J71" t="s">
-        <v>62</v>
+        <v>119</v>
       </c>
       <c r="K71" t="s">
-        <v>63</v>
+        <v>120</v>
       </c>
       <c r="L71" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="N71" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="O71" t="s">
         <v>34</v>
@@ -6252,13 +6300,13 @@
         <v>0</v>
       </c>
       <c r="S71" s="1">
-        <v>5322.29</v>
+        <v>93824</v>
       </c>
       <c r="T71" s="1">
-        <v>691.9</v>
+        <v>0</v>
       </c>
       <c r="U71" s="1">
-        <v>6014.19</v>
+        <v>93824</v>
       </c>
       <c r="V71" t="s">
         <v>35</v>
@@ -6267,7 +6315,7 @@
         <v>1</v>
       </c>
       <c r="X71">
-        <v>6014.19</v>
+        <v>93824</v>
       </c>
     </row>
     <row r="72" spans="1:24">
@@ -6281,7 +6329,7 @@
         <v>289</v>
       </c>
       <c r="D72" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E72" t="s">
         <v>290</v>
@@ -6296,16 +6344,16 @@
         <v>30</v>
       </c>
       <c r="J72" t="s">
-        <v>119</v>
+        <v>56</v>
       </c>
       <c r="K72" t="s">
-        <v>120</v>
+        <v>57</v>
       </c>
       <c r="L72" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="N72" t="s">
-        <v>91</v>
+        <v>126</v>
       </c>
       <c r="O72" t="s">
         <v>34</v>
@@ -6317,13 +6365,13 @@
         <v>0</v>
       </c>
       <c r="S72" s="1">
-        <v>93824</v>
+        <v>32872.99</v>
       </c>
       <c r="T72" s="1">
-        <v>0</v>
+        <v>4468.4882799999996</v>
       </c>
       <c r="U72" s="1">
-        <v>93824</v>
+        <v>37341.478280000003</v>
       </c>
       <c r="V72" t="s">
         <v>35</v>
@@ -6332,7 +6380,7 @@
         <v>1</v>
       </c>
       <c r="X72">
-        <v>93824</v>
+        <v>37341.478280000003</v>
       </c>
     </row>
     <row r="73" spans="1:24">
@@ -6346,7 +6394,7 @@
         <v>291</v>
       </c>
       <c r="D73" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E73" t="s">
         <v>292</v>
@@ -6361,16 +6409,16 @@
         <v>30</v>
       </c>
       <c r="J73" t="s">
-        <v>56</v>
+        <v>293</v>
       </c>
       <c r="K73" t="s">
-        <v>57</v>
+        <v>294</v>
       </c>
       <c r="L73" t="s">
-        <v>58</v>
+        <v>295</v>
       </c>
       <c r="N73" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="O73" t="s">
         <v>34</v>
@@ -6382,13 +6430,13 @@
         <v>0</v>
       </c>
       <c r="S73" s="1">
-        <v>32872.99</v>
+        <v>70000</v>
       </c>
       <c r="T73" s="1">
-        <v>4468.4882799999996</v>
+        <v>0</v>
       </c>
       <c r="U73" s="1">
-        <v>37341.478280000003</v>
+        <v>70000</v>
       </c>
       <c r="V73" t="s">
         <v>35</v>
@@ -6397,7 +6445,7 @@
         <v>1</v>
       </c>
       <c r="X73">
-        <v>37341.478280000003</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="74" spans="1:24">
@@ -6408,13 +6456,13 @@
         <v>24</v>
       </c>
       <c r="C74" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="D74" t="s">
         <v>66</v>
       </c>
       <c r="E74" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="F74" t="s">
         <v>28</v>
@@ -6426,16 +6474,16 @@
         <v>30</v>
       </c>
       <c r="J74" t="s">
-        <v>295</v>
+        <v>68</v>
       </c>
       <c r="K74" t="s">
-        <v>296</v>
+        <v>69</v>
       </c>
       <c r="L74" t="s">
-        <v>297</v>
+        <v>70</v>
       </c>
       <c r="N74" t="s">
-        <v>129</v>
+        <v>71</v>
       </c>
       <c r="O74" t="s">
         <v>34</v>
@@ -6447,13 +6495,13 @@
         <v>0</v>
       </c>
       <c r="S74" s="1">
-        <v>70000</v>
+        <v>580983</v>
       </c>
       <c r="T74" s="1">
-        <v>0</v>
+        <v>75527.789999999994</v>
       </c>
       <c r="U74" s="1">
-        <v>70000</v>
+        <v>656510.79</v>
       </c>
       <c r="V74" t="s">
         <v>35</v>
@@ -6462,7 +6510,7 @@
         <v>1</v>
       </c>
       <c r="X74">
-        <v>70000</v>
+        <v>656510.79</v>
       </c>
     </row>
     <row r="75" spans="1:24">
@@ -6476,7 +6524,7 @@
         <v>298</v>
       </c>
       <c r="D75" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="E75" t="s">
         <v>299</v>
@@ -6491,16 +6539,16 @@
         <v>30</v>
       </c>
       <c r="J75" t="s">
-        <v>68</v>
+        <v>229</v>
       </c>
       <c r="K75" t="s">
-        <v>69</v>
+        <v>230</v>
       </c>
       <c r="L75" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="N75" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="O75" t="s">
         <v>34</v>
@@ -6512,13 +6560,13 @@
         <v>0</v>
       </c>
       <c r="S75" s="1">
-        <v>580983</v>
+        <v>11900</v>
       </c>
       <c r="T75" s="1">
-        <v>75527.789999999994</v>
+        <v>1222</v>
       </c>
       <c r="U75" s="1">
-        <v>656510.79</v>
+        <v>13122</v>
       </c>
       <c r="V75" t="s">
         <v>35</v>
@@ -6527,7 +6575,7 @@
         <v>1</v>
       </c>
       <c r="X75">
-        <v>656510.79</v>
+        <v>13122</v>
       </c>
     </row>
     <row r="76" spans="1:24">
@@ -6541,7 +6589,7 @@
         <v>300</v>
       </c>
       <c r="D76" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="E76" t="s">
         <v>301</v>
@@ -6556,16 +6604,16 @@
         <v>30</v>
       </c>
       <c r="J76" t="s">
-        <v>229</v>
+        <v>62</v>
       </c>
       <c r="K76" t="s">
-        <v>230</v>
+        <v>63</v>
       </c>
       <c r="L76" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="N76" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="O76" t="s">
         <v>34</v>
@@ -6577,13 +6625,13 @@
         <v>0</v>
       </c>
       <c r="S76" s="1">
-        <v>11900</v>
+        <v>8956.11</v>
       </c>
       <c r="T76" s="1">
-        <v>1222</v>
+        <v>1164.3</v>
       </c>
       <c r="U76" s="1">
-        <v>13122</v>
+        <v>10120.41</v>
       </c>
       <c r="V76" t="s">
         <v>35</v>
@@ -6592,7 +6640,7 @@
         <v>1</v>
       </c>
       <c r="X76">
-        <v>13122</v>
+        <v>10120.41</v>
       </c>
     </row>
     <row r="77" spans="1:24">
@@ -6606,7 +6654,7 @@
         <v>302</v>
       </c>
       <c r="D77" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E77" t="s">
         <v>303</v>
@@ -6621,16 +6669,16 @@
         <v>30</v>
       </c>
       <c r="J77" t="s">
-        <v>62</v>
+        <v>304</v>
       </c>
       <c r="K77" t="s">
-        <v>63</v>
+        <v>305</v>
       </c>
       <c r="L77" t="s">
         <v>64</v>
       </c>
       <c r="N77" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="O77" t="s">
         <v>34</v>
@@ -6642,13 +6690,13 @@
         <v>0</v>
       </c>
       <c r="S77" s="1">
-        <v>8956.11</v>
+        <v>353.98230000000001</v>
       </c>
       <c r="T77" s="1">
-        <v>1164.3</v>
+        <v>46.017699999999998</v>
       </c>
       <c r="U77" s="1">
-        <v>10120.41</v>
+        <v>400</v>
       </c>
       <c r="V77" t="s">
         <v>35</v>
@@ -6657,7 +6705,7 @@
         <v>1</v>
       </c>
       <c r="X77">
-        <v>10120.41</v>
+        <v>400</v>
       </c>
     </row>
     <row r="78" spans="1:24">
@@ -6668,13 +6716,13 @@
         <v>24</v>
       </c>
       <c r="C78" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="D78" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E78" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="F78" t="s">
         <v>28</v>
@@ -6686,16 +6734,16 @@
         <v>30</v>
       </c>
       <c r="J78" t="s">
-        <v>306</v>
+        <v>39</v>
       </c>
       <c r="K78" t="s">
-        <v>307</v>
+        <v>40</v>
       </c>
       <c r="L78" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="N78" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="O78" t="s">
         <v>34</v>
@@ -6707,13 +6755,13 @@
         <v>0</v>
       </c>
       <c r="S78" s="1">
-        <v>353.98230000000001</v>
+        <v>140000</v>
       </c>
       <c r="T78" s="1">
-        <v>46.017699999999998</v>
+        <v>18200</v>
       </c>
       <c r="U78" s="1">
-        <v>400</v>
+        <v>158200</v>
       </c>
       <c r="V78" t="s">
         <v>35</v>
@@ -6722,7 +6770,7 @@
         <v>1</v>
       </c>
       <c r="X78">
-        <v>400</v>
+        <v>158200</v>
       </c>
     </row>
     <row r="79" spans="1:24">
@@ -6736,7 +6784,7 @@
         <v>308</v>
       </c>
       <c r="D79" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="E79" t="s">
         <v>309</v>
@@ -6751,16 +6799,16 @@
         <v>30</v>
       </c>
       <c r="J79" t="s">
-        <v>39</v>
+        <v>310</v>
       </c>
       <c r="K79" t="s">
-        <v>40</v>
+        <v>311</v>
       </c>
       <c r="L79" t="s">
-        <v>41</v>
+        <v>282</v>
       </c>
       <c r="N79" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="O79" t="s">
         <v>34</v>
@@ -6772,13 +6820,13 @@
         <v>0</v>
       </c>
       <c r="S79" s="1">
-        <v>140000</v>
+        <v>47639.822999999997</v>
       </c>
       <c r="T79" s="1">
-        <v>18200</v>
+        <v>6193.1769999999997</v>
       </c>
       <c r="U79" s="1">
-        <v>158200</v>
+        <v>53833</v>
       </c>
       <c r="V79" t="s">
         <v>35</v>
@@ -6787,7 +6835,7 @@
         <v>1</v>
       </c>
       <c r="X79">
-        <v>158200</v>
+        <v>53833</v>
       </c>
     </row>
     <row r="80" spans="1:24">
@@ -6798,35 +6846,35 @@
         <v>24</v>
       </c>
       <c r="C80" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D80" t="s">
+        <v>101</v>
+      </c>
+      <c r="E80" t="s">
+        <v>313</v>
+      </c>
+      <c r="F80" t="s">
+        <v>28</v>
+      </c>
+      <c r="G80" t="s">
+        <v>29</v>
+      </c>
+      <c r="H80" t="s">
+        <v>30</v>
+      </c>
+      <c r="J80" t="s">
+        <v>314</v>
+      </c>
+      <c r="K80" t="s">
+        <v>315</v>
+      </c>
+      <c r="L80" t="s">
+        <v>155</v>
+      </c>
+      <c r="N80" t="s">
         <v>60</v>
       </c>
-      <c r="E80" t="s">
-        <v>311</v>
-      </c>
-      <c r="F80" t="s">
-        <v>28</v>
-      </c>
-      <c r="G80" t="s">
-        <v>29</v>
-      </c>
-      <c r="H80" t="s">
-        <v>30</v>
-      </c>
-      <c r="J80" t="s">
-        <v>312</v>
-      </c>
-      <c r="K80" t="s">
-        <v>313</v>
-      </c>
-      <c r="L80" t="s">
-        <v>284</v>
-      </c>
-      <c r="N80" t="s">
-        <v>54</v>
-      </c>
       <c r="O80" t="s">
         <v>34</v>
       </c>
@@ -6837,13 +6885,13 @@
         <v>0</v>
       </c>
       <c r="S80" s="1">
-        <v>47639.822999999997</v>
+        <v>6615</v>
       </c>
       <c r="T80" s="1">
-        <v>6193.1769999999997</v>
+        <v>0</v>
       </c>
       <c r="U80" s="1">
-        <v>53833</v>
+        <v>6615</v>
       </c>
       <c r="V80" t="s">
         <v>35</v>
@@ -6852,7 +6900,7 @@
         <v>1</v>
       </c>
       <c r="X80">
-        <v>53833</v>
+        <v>6615</v>
       </c>
     </row>
     <row r="81" spans="1:24">
@@ -6863,13 +6911,13 @@
         <v>24</v>
       </c>
       <c r="C81" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D81" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="E81" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="F81" t="s">
         <v>28</v>
@@ -6881,16 +6929,16 @@
         <v>30</v>
       </c>
       <c r="J81" t="s">
-        <v>316</v>
+        <v>68</v>
       </c>
       <c r="K81" t="s">
-        <v>317</v>
+        <v>69</v>
       </c>
       <c r="L81" t="s">
-        <v>155</v>
+        <v>70</v>
       </c>
       <c r="N81" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="O81" t="s">
         <v>34</v>
@@ -6902,13 +6950,13 @@
         <v>0</v>
       </c>
       <c r="S81" s="1">
-        <v>6615</v>
+        <v>1067583.1100000001</v>
       </c>
       <c r="T81" s="1">
-        <v>0</v>
+        <v>138785.79999999999</v>
       </c>
       <c r="U81" s="1">
-        <v>6615</v>
+        <v>1206368.9099999999</v>
       </c>
       <c r="V81" t="s">
         <v>35</v>
@@ -6917,7 +6965,7 @@
         <v>1</v>
       </c>
       <c r="X81">
-        <v>6615</v>
+        <v>1206368.9099999999</v>
       </c>
     </row>
     <row r="82" spans="1:24">
@@ -6931,7 +6979,7 @@
         <v>318</v>
       </c>
       <c r="D82" t="s">
-        <v>66</v>
+        <v>234</v>
       </c>
       <c r="E82" t="s">
         <v>319</v>
@@ -6946,16 +6994,16 @@
         <v>30</v>
       </c>
       <c r="J82" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="K82" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="L82" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="N82" t="s">
-        <v>71</v>
+        <v>234</v>
       </c>
       <c r="O82" t="s">
         <v>34</v>
@@ -6967,13 +7015,13 @@
         <v>0</v>
       </c>
       <c r="S82" s="1">
-        <v>1067583.1100000001</v>
+        <v>9857.94</v>
       </c>
       <c r="T82" s="1">
-        <v>138785.79999999999</v>
+        <v>1281.53</v>
       </c>
       <c r="U82" s="1">
-        <v>1206368.9099999999</v>
+        <v>11139.47</v>
       </c>
       <c r="V82" t="s">
         <v>35</v>
@@ -6982,7 +7030,7 @@
         <v>1</v>
       </c>
       <c r="X82">
-        <v>1206368.9099999999</v>
+        <v>11139.47</v>
       </c>
     </row>
     <row r="83" spans="1:24">
@@ -6996,7 +7044,7 @@
         <v>320</v>
       </c>
       <c r="D83" t="s">
-        <v>234</v>
+        <v>37</v>
       </c>
       <c r="E83" t="s">
         <v>321</v>
@@ -7011,16 +7059,16 @@
         <v>30</v>
       </c>
       <c r="J83" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="K83" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="L83" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="N83" t="s">
-        <v>234</v>
+        <v>42</v>
       </c>
       <c r="O83" t="s">
         <v>34</v>
@@ -7032,13 +7080,13 @@
         <v>0</v>
       </c>
       <c r="S83" s="1">
-        <v>9857.94</v>
+        <v>7500</v>
       </c>
       <c r="T83" s="1">
-        <v>1281.53</v>
+        <v>0</v>
       </c>
       <c r="U83" s="1">
-        <v>11139.47</v>
+        <v>7500</v>
       </c>
       <c r="V83" t="s">
         <v>35</v>
@@ -7047,7 +7095,7 @@
         <v>1</v>
       </c>
       <c r="X83">
-        <v>11139.47</v>
+        <v>7500</v>
       </c>
     </row>
     <row r="84" spans="1:24">
@@ -7055,13 +7103,13 @@
         <v>39015</v>
       </c>
       <c r="B84" t="s">
-        <v>24</v>
+        <v>121</v>
       </c>
       <c r="C84" t="s">
         <v>322</v>
       </c>
       <c r="D84" t="s">
-        <v>37</v>
+        <v>242</v>
       </c>
       <c r="E84" t="s">
         <v>323</v>
@@ -7076,16 +7124,16 @@
         <v>30</v>
       </c>
       <c r="J84" t="s">
-        <v>31</v>
+        <v>169</v>
       </c>
       <c r="K84" t="s">
-        <v>32</v>
+        <v>170</v>
       </c>
       <c r="L84" t="s">
-        <v>33</v>
+        <v>171</v>
       </c>
       <c r="N84" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="O84" t="s">
         <v>34</v>
@@ -7097,13 +7145,13 @@
         <v>0</v>
       </c>
       <c r="S84" s="1">
-        <v>7500</v>
+        <v>7079.6459999999997</v>
       </c>
       <c r="T84" s="1">
-        <v>0</v>
+        <v>920.35400000000004</v>
       </c>
       <c r="U84" s="1">
-        <v>7500</v>
+        <v>8000</v>
       </c>
       <c r="V84" t="s">
         <v>35</v>
@@ -7112,7 +7160,7 @@
         <v>1</v>
       </c>
       <c r="X84">
-        <v>7500</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="85" spans="1:24">
@@ -7120,13 +7168,13 @@
         <v>39015</v>
       </c>
       <c r="B85" t="s">
-        <v>121</v>
+        <v>24</v>
       </c>
       <c r="C85" t="s">
         <v>324</v>
       </c>
       <c r="D85" t="s">
-        <v>242</v>
+        <v>44</v>
       </c>
       <c r="E85" t="s">
         <v>325</v>
@@ -7141,16 +7189,16 @@
         <v>30</v>
       </c>
       <c r="J85" t="s">
-        <v>169</v>
+        <v>105</v>
       </c>
       <c r="K85" t="s">
-        <v>170</v>
+        <v>106</v>
       </c>
       <c r="L85" t="s">
-        <v>171</v>
+        <v>107</v>
       </c>
       <c r="N85" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="O85" t="s">
         <v>34</v>
@@ -7162,13 +7210,13 @@
         <v>0</v>
       </c>
       <c r="S85" s="1">
-        <v>7079.6459999999997</v>
+        <v>12440.708280000001</v>
       </c>
       <c r="T85" s="1">
-        <v>920.35400000000004</v>
+        <v>1617.2920799999999</v>
       </c>
       <c r="U85" s="1">
-        <v>8000</v>
+        <v>14058.00036</v>
       </c>
       <c r="V85" t="s">
         <v>35</v>
@@ -7177,7 +7225,7 @@
         <v>1</v>
       </c>
       <c r="X85">
-        <v>8000</v>
+        <v>14058.00036</v>
       </c>
     </row>
     <row r="86" spans="1:24">
@@ -7191,7 +7239,7 @@
         <v>326</v>
       </c>
       <c r="D86" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="E86" t="s">
         <v>327</v>
@@ -7206,16 +7254,16 @@
         <v>30</v>
       </c>
       <c r="J86" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="K86" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="L86" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="N86" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="O86" t="s">
         <v>34</v>
@@ -7227,13 +7275,13 @@
         <v>0</v>
       </c>
       <c r="S86" s="1">
-        <v>12440.708280000001</v>
+        <v>93824</v>
       </c>
       <c r="T86" s="1">
-        <v>1617.2920799999999</v>
+        <v>0</v>
       </c>
       <c r="U86" s="1">
-        <v>14058.00036</v>
+        <v>93824</v>
       </c>
       <c r="V86" t="s">
         <v>35</v>
@@ -7242,7 +7290,7 @@
         <v>1</v>
       </c>
       <c r="X86">
-        <v>14058.00036</v>
+        <v>93824</v>
       </c>
     </row>
     <row r="87" spans="1:24">
@@ -7256,7 +7304,7 @@
         <v>328</v>
       </c>
       <c r="D87" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E87" t="s">
         <v>329</v>
@@ -7271,16 +7319,16 @@
         <v>30</v>
       </c>
       <c r="J87" t="s">
-        <v>119</v>
+        <v>247</v>
       </c>
       <c r="K87" t="s">
-        <v>120</v>
+        <v>248</v>
       </c>
       <c r="L87" t="s">
-        <v>76</v>
+        <v>249</v>
       </c>
       <c r="N87" t="s">
-        <v>91</v>
+        <v>126</v>
       </c>
       <c r="O87" t="s">
         <v>34</v>
@@ -7292,13 +7340,13 @@
         <v>0</v>
       </c>
       <c r="S87" s="1">
-        <v>93824</v>
+        <v>30598.039219999999</v>
       </c>
       <c r="T87" s="1">
-        <v>0</v>
+        <v>611.96078</v>
       </c>
       <c r="U87" s="1">
-        <v>93824</v>
+        <v>31210</v>
       </c>
       <c r="V87" t="s">
         <v>35</v>
@@ -7307,7 +7355,7 @@
         <v>1</v>
       </c>
       <c r="X87">
-        <v>93824</v>
+        <v>31210</v>
       </c>
     </row>
     <row r="88" spans="1:24">
@@ -7321,7 +7369,7 @@
         <v>330</v>
       </c>
       <c r="D88" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E88" t="s">
         <v>331</v>
@@ -7336,16 +7384,16 @@
         <v>30</v>
       </c>
       <c r="J88" t="s">
-        <v>249</v>
+        <v>332</v>
       </c>
       <c r="K88" t="s">
-        <v>250</v>
+        <v>333</v>
       </c>
       <c r="L88" t="s">
-        <v>251</v>
+        <v>282</v>
       </c>
       <c r="N88" t="s">
-        <v>126</v>
+        <v>71</v>
       </c>
       <c r="O88" t="s">
         <v>34</v>
@@ -7357,13 +7405,13 @@
         <v>0</v>
       </c>
       <c r="S88" s="1">
-        <v>30598.039219999999</v>
+        <v>65626.2</v>
       </c>
       <c r="T88" s="1">
-        <v>611.96078</v>
+        <v>8210.18</v>
       </c>
       <c r="U88" s="1">
-        <v>31210</v>
+        <v>73836.38</v>
       </c>
       <c r="V88" t="s">
         <v>35</v>
@@ -7372,7 +7420,7 @@
         <v>1</v>
       </c>
       <c r="X88">
-        <v>31210</v>
+        <v>73836.38</v>
       </c>
     </row>
     <row r="89" spans="1:24">
@@ -7383,13 +7431,13 @@
         <v>24</v>
       </c>
       <c r="C89" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="D89" t="s">
         <v>66</v>
       </c>
       <c r="E89" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="F89" t="s">
         <v>28</v>
@@ -7401,16 +7449,16 @@
         <v>30</v>
       </c>
       <c r="J89" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="K89" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="L89" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="N89" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="O89" t="s">
         <v>34</v>
@@ -7422,13 +7470,13 @@
         <v>0</v>
       </c>
       <c r="S89" s="1">
-        <v>65626.2</v>
+        <v>6814</v>
       </c>
       <c r="T89" s="1">
-        <v>8210.18</v>
+        <v>885.82</v>
       </c>
       <c r="U89" s="1">
-        <v>73836.38</v>
+        <v>7699.82</v>
       </c>
       <c r="V89" t="s">
         <v>35</v>
@@ -7437,7 +7485,7 @@
         <v>1</v>
       </c>
       <c r="X89">
-        <v>73836.38</v>
+        <v>7699.82</v>
       </c>
     </row>
     <row r="90" spans="1:24">
@@ -7448,13 +7496,13 @@
         <v>24</v>
       </c>
       <c r="C90" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="D90" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="E90" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="F90" t="s">
         <v>28</v>
@@ -7466,16 +7514,16 @@
         <v>30</v>
       </c>
       <c r="J90" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="K90" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="L90" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="N90" t="s">
-        <v>101</v>
+        <v>26</v>
       </c>
       <c r="O90" t="s">
         <v>34</v>
@@ -7487,13 +7535,13 @@
         <v>0</v>
       </c>
       <c r="S90" s="1">
-        <v>6814</v>
+        <v>2654.87</v>
       </c>
       <c r="T90" s="1">
-        <v>885.82</v>
+        <v>345.13310000000001</v>
       </c>
       <c r="U90" s="1">
-        <v>7699.82</v>
+        <v>3000.0030999999999</v>
       </c>
       <c r="V90" t="s">
         <v>35</v>
@@ -7502,7 +7550,7 @@
         <v>1</v>
       </c>
       <c r="X90">
-        <v>7699.82</v>
+        <v>3000.0030999999999</v>
       </c>
     </row>
     <row r="91" spans="1:24">
@@ -7513,13 +7561,13 @@
         <v>24</v>
       </c>
       <c r="C91" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D91" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="E91" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="F91" t="s">
         <v>28</v>
@@ -7531,16 +7579,16 @@
         <v>30</v>
       </c>
       <c r="J91" t="s">
-        <v>342</v>
+        <v>119</v>
       </c>
       <c r="K91" t="s">
-        <v>343</v>
+        <v>120</v>
       </c>
       <c r="L91" t="s">
-        <v>284</v>
+        <v>76</v>
       </c>
       <c r="N91" t="s">
-        <v>26</v>
+        <v>172</v>
       </c>
       <c r="O91" t="s">
         <v>34</v>
@@ -7552,13 +7600,13 @@
         <v>0</v>
       </c>
       <c r="S91" s="1">
-        <v>2654.87</v>
+        <v>121002</v>
       </c>
       <c r="T91" s="1">
-        <v>345.13310000000001</v>
+        <v>0</v>
       </c>
       <c r="U91" s="1">
-        <v>3000.0030999999999</v>
+        <v>121002</v>
       </c>
       <c r="V91" t="s">
         <v>35</v>
@@ -7567,7 +7615,7 @@
         <v>1</v>
       </c>
       <c r="X91">
-        <v>3000.0030999999999</v>
+        <v>121002</v>
       </c>
     </row>
     <row r="92" spans="1:24">
@@ -7581,7 +7629,7 @@
         <v>344</v>
       </c>
       <c r="D92" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="E92" t="s">
         <v>345</v>
@@ -7596,16 +7644,16 @@
         <v>30</v>
       </c>
       <c r="J92" t="s">
-        <v>119</v>
+        <v>175</v>
       </c>
       <c r="K92" t="s">
-        <v>120</v>
+        <v>176</v>
       </c>
       <c r="L92" t="s">
-        <v>76</v>
+        <v>33</v>
       </c>
       <c r="N92" t="s">
-        <v>172</v>
+        <v>49</v>
       </c>
       <c r="O92" t="s">
         <v>34</v>
@@ -7617,13 +7665,13 @@
         <v>0</v>
       </c>
       <c r="S92" s="1">
-        <v>121002</v>
+        <v>14163.74</v>
       </c>
       <c r="T92" s="1">
-        <v>0</v>
+        <v>1673.8969</v>
       </c>
       <c r="U92" s="1">
-        <v>121002</v>
+        <v>15837.6369</v>
       </c>
       <c r="V92" t="s">
         <v>35</v>
@@ -7632,7 +7680,7 @@
         <v>1</v>
       </c>
       <c r="X92">
-        <v>121002</v>
+        <v>15837.6369</v>
       </c>
     </row>
     <row r="93" spans="1:24">
@@ -7646,7 +7694,7 @@
         <v>346</v>
       </c>
       <c r="D93" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E93" t="s">
         <v>347</v>
@@ -7661,16 +7709,16 @@
         <v>30</v>
       </c>
       <c r="J93" t="s">
-        <v>175</v>
+        <v>83</v>
       </c>
       <c r="K93" t="s">
-        <v>176</v>
+        <v>84</v>
       </c>
       <c r="L93" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="N93" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="O93" t="s">
         <v>34</v>
@@ -7682,13 +7730,13 @@
         <v>0</v>
       </c>
       <c r="S93" s="1">
-        <v>14163.74</v>
+        <v>19999.999970000001</v>
       </c>
       <c r="T93" s="1">
-        <v>1673.8969</v>
+        <v>0</v>
       </c>
       <c r="U93" s="1">
-        <v>15837.6369</v>
+        <v>19999.999970000001</v>
       </c>
       <c r="V93" t="s">
         <v>35</v>
@@ -7697,7 +7745,7 @@
         <v>1</v>
       </c>
       <c r="X93">
-        <v>15837.6369</v>
+        <v>19999.999970000001</v>
       </c>
     </row>
     <row r="94" spans="1:24">
@@ -7711,7 +7759,7 @@
         <v>348</v>
       </c>
       <c r="D94" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="E94" t="s">
         <v>349</v>
@@ -7726,16 +7774,16 @@
         <v>30</v>
       </c>
       <c r="J94" t="s">
-        <v>83</v>
+        <v>215</v>
       </c>
       <c r="K94" t="s">
-        <v>84</v>
+        <v>216</v>
       </c>
       <c r="L94" t="s">
-        <v>76</v>
+        <v>217</v>
       </c>
       <c r="N94" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="O94" t="s">
         <v>34</v>
@@ -7747,13 +7795,13 @@
         <v>0</v>
       </c>
       <c r="S94" s="1">
-        <v>19999.999970000001</v>
+        <v>39823.01</v>
       </c>
       <c r="T94" s="1">
-        <v>0</v>
+        <v>5176.9912999999997</v>
       </c>
       <c r="U94" s="1">
-        <v>19999.999970000001</v>
+        <v>45000.001300000004</v>
       </c>
       <c r="V94" t="s">
         <v>35</v>
@@ -7762,7 +7810,7 @@
         <v>1</v>
       </c>
       <c r="X94">
-        <v>19999.999970000001</v>
+        <v>45000.001300000004</v>
       </c>
     </row>
     <row r="95" spans="1:24">
@@ -7776,7 +7824,7 @@
         <v>350</v>
       </c>
       <c r="D95" t="s">
-        <v>60</v>
+        <v>101</v>
       </c>
       <c r="E95" t="s">
         <v>351</v>
@@ -7791,16 +7839,16 @@
         <v>30</v>
       </c>
       <c r="J95" t="s">
-        <v>215</v>
+        <v>46</v>
       </c>
       <c r="K95" t="s">
-        <v>216</v>
+        <v>47</v>
       </c>
       <c r="L95" t="s">
-        <v>217</v>
+        <v>48</v>
       </c>
       <c r="N95" t="s">
-        <v>54</v>
+        <v>101</v>
       </c>
       <c r="O95" t="s">
         <v>34</v>
@@ -7812,13 +7860,13 @@
         <v>0</v>
       </c>
       <c r="S95" s="1">
-        <v>39823.01</v>
+        <v>6392.85</v>
       </c>
       <c r="T95" s="1">
-        <v>5176.9912999999997</v>
+        <v>831.07</v>
       </c>
       <c r="U95" s="1">
-        <v>45000.001300000004</v>
+        <v>7223.92</v>
       </c>
       <c r="V95" t="s">
         <v>35</v>
@@ -7827,7 +7875,7 @@
         <v>1</v>
       </c>
       <c r="X95">
-        <v>45000.001300000004</v>
+        <v>7223.92</v>
       </c>
     </row>
     <row r="96" spans="1:24">
@@ -7841,7 +7889,7 @@
         <v>352</v>
       </c>
       <c r="D96" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="E96" t="s">
         <v>353</v>
@@ -7856,16 +7904,16 @@
         <v>30</v>
       </c>
       <c r="J96" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="K96" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="L96" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="N96" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="O96" t="s">
         <v>34</v>
@@ -7877,13 +7925,13 @@
         <v>0</v>
       </c>
       <c r="S96" s="1">
-        <v>6392.85</v>
+        <v>460544</v>
       </c>
       <c r="T96" s="1">
-        <v>831.07</v>
+        <v>59870.720000000001</v>
       </c>
       <c r="U96" s="1">
-        <v>7223.92</v>
+        <v>520414.71999999997</v>
       </c>
       <c r="V96" t="s">
         <v>35</v>
@@ -7892,7 +7940,7 @@
         <v>1</v>
       </c>
       <c r="X96">
-        <v>7223.92</v>
+        <v>520414.71999999997</v>
       </c>
     </row>
     <row r="97" spans="1:24">
@@ -7906,7 +7954,7 @@
         <v>354</v>
       </c>
       <c r="D97" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="E97" t="s">
         <v>355</v>
@@ -7921,16 +7969,16 @@
         <v>30</v>
       </c>
       <c r="J97" t="s">
-        <v>68</v>
+        <v>119</v>
       </c>
       <c r="K97" t="s">
-        <v>69</v>
+        <v>120</v>
       </c>
       <c r="L97" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="N97" t="s">
-        <v>71</v>
+        <v>234</v>
       </c>
       <c r="O97" t="s">
         <v>34</v>
@@ -7942,13 +7990,13 @@
         <v>0</v>
       </c>
       <c r="S97" s="1">
-        <v>460544</v>
+        <v>29631</v>
       </c>
       <c r="T97" s="1">
-        <v>59870.720000000001</v>
+        <v>0</v>
       </c>
       <c r="U97" s="1">
-        <v>520414.71999999997</v>
+        <v>29631</v>
       </c>
       <c r="V97" t="s">
         <v>35</v>
@@ -7957,7 +8005,7 @@
         <v>1</v>
       </c>
       <c r="X97">
-        <v>520414.71999999997</v>
+        <v>29631</v>
       </c>
     </row>
     <row r="98" spans="1:24">
@@ -7971,7 +8019,7 @@
         <v>356</v>
       </c>
       <c r="D98" t="s">
-        <v>103</v>
+        <v>37</v>
       </c>
       <c r="E98" t="s">
         <v>357</v>
@@ -7986,16 +8034,16 @@
         <v>30</v>
       </c>
       <c r="J98" t="s">
-        <v>119</v>
+        <v>62</v>
       </c>
       <c r="K98" t="s">
-        <v>120</v>
+        <v>63</v>
       </c>
       <c r="L98" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="N98" t="s">
-        <v>234</v>
+        <v>42</v>
       </c>
       <c r="O98" t="s">
         <v>34</v>
@@ -8007,13 +8055,13 @@
         <v>0</v>
       </c>
       <c r="S98" s="1">
-        <v>29631</v>
+        <v>10548.72</v>
       </c>
       <c r="T98" s="1">
-        <v>0</v>
+        <v>1371.33</v>
       </c>
       <c r="U98" s="1">
-        <v>29631</v>
+        <v>11920.05</v>
       </c>
       <c r="V98" t="s">
         <v>35</v>
@@ -8022,7 +8070,7 @@
         <v>1</v>
       </c>
       <c r="X98">
-        <v>29631</v>
+        <v>11920.05</v>
       </c>
     </row>
     <row r="99" spans="1:24">
@@ -8036,7 +8084,7 @@
         <v>358</v>
       </c>
       <c r="D99" t="s">
-        <v>37</v>
+        <v>112</v>
       </c>
       <c r="E99" t="s">
         <v>359</v>
@@ -8051,16 +8099,16 @@
         <v>30</v>
       </c>
       <c r="J99" t="s">
-        <v>62</v>
+        <v>138</v>
       </c>
       <c r="K99" t="s">
-        <v>63</v>
+        <v>139</v>
       </c>
       <c r="L99" t="s">
-        <v>64</v>
+        <v>140</v>
       </c>
       <c r="N99" t="s">
-        <v>42</v>
+        <v>242</v>
       </c>
       <c r="O99" t="s">
         <v>34</v>
@@ -8072,13 +8120,13 @@
         <v>0</v>
       </c>
       <c r="S99" s="1">
-        <v>10548.72</v>
+        <v>989900.12</v>
       </c>
       <c r="T99" s="1">
-        <v>1371.33</v>
+        <v>12816.8092</v>
       </c>
       <c r="U99" s="1">
-        <v>11920.05</v>
+        <v>1002716.9292</v>
       </c>
       <c r="V99" t="s">
         <v>35</v>
@@ -8087,7 +8135,7 @@
         <v>1</v>
       </c>
       <c r="X99">
-        <v>11920.05</v>
+        <v>1002716.9292</v>
       </c>
     </row>
     <row r="100" spans="1:24">
@@ -8101,7 +8149,7 @@
         <v>360</v>
       </c>
       <c r="D100" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E100" t="s">
         <v>361</v>
@@ -8116,16 +8164,16 @@
         <v>30</v>
       </c>
       <c r="J100" t="s">
-        <v>138</v>
+        <v>340</v>
       </c>
       <c r="K100" t="s">
-        <v>139</v>
+        <v>341</v>
       </c>
       <c r="L100" t="s">
-        <v>140</v>
+        <v>282</v>
       </c>
       <c r="N100" t="s">
-        <v>242</v>
+        <v>44</v>
       </c>
       <c r="O100" t="s">
         <v>34</v>
@@ -8137,13 +8185,13 @@
         <v>0</v>
       </c>
       <c r="S100" s="1">
-        <v>989900.12</v>
+        <v>2477.88</v>
       </c>
       <c r="T100" s="1">
-        <v>12816.8092</v>
+        <v>322.12439999999998</v>
       </c>
       <c r="U100" s="1">
-        <v>1002716.9292</v>
+        <v>2800.0043999999998</v>
       </c>
       <c r="V100" t="s">
         <v>35</v>
@@ -8152,7 +8200,7 @@
         <v>1</v>
       </c>
       <c r="X100">
-        <v>1002716.9292</v>
+        <v>2800.0043999999998</v>
       </c>
     </row>
     <row r="101" spans="1:24">
@@ -8166,7 +8214,7 @@
         <v>362</v>
       </c>
       <c r="D101" t="s">
-        <v>117</v>
+        <v>54</v>
       </c>
       <c r="E101" t="s">
         <v>363</v>
@@ -8181,16 +8229,16 @@
         <v>30</v>
       </c>
       <c r="J101" t="s">
-        <v>342</v>
+        <v>119</v>
       </c>
       <c r="K101" t="s">
-        <v>343</v>
+        <v>120</v>
       </c>
       <c r="L101" t="s">
-        <v>284</v>
+        <v>76</v>
       </c>
       <c r="N101" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="O101" t="s">
         <v>34</v>
@@ -8202,13 +8250,13 @@
         <v>0</v>
       </c>
       <c r="S101" s="1">
-        <v>2477.88</v>
+        <v>93824</v>
       </c>
       <c r="T101" s="1">
-        <v>322.12439999999998</v>
+        <v>0</v>
       </c>
       <c r="U101" s="1">
-        <v>2800.0043999999998</v>
+        <v>93824</v>
       </c>
       <c r="V101" t="s">
         <v>35</v>
@@ -8217,7 +8265,7 @@
         <v>1</v>
       </c>
       <c r="X101">
-        <v>2800.0043999999998</v>
+        <v>93824</v>
       </c>
     </row>
     <row r="102" spans="1:24">
@@ -8231,7 +8279,7 @@
         <v>364</v>
       </c>
       <c r="D102" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E102" t="s">
         <v>365</v>
@@ -8246,16 +8294,16 @@
         <v>30</v>
       </c>
       <c r="J102" t="s">
-        <v>119</v>
+        <v>366</v>
       </c>
       <c r="K102" t="s">
-        <v>120</v>
+        <v>367</v>
       </c>
       <c r="L102" t="s">
-        <v>76</v>
+        <v>368</v>
       </c>
       <c r="N102" t="s">
-        <v>91</v>
+        <v>126</v>
       </c>
       <c r="O102" t="s">
         <v>34</v>
@@ -8267,13 +8315,13 @@
         <v>0</v>
       </c>
       <c r="S102" s="1">
-        <v>93824</v>
+        <v>102654.78</v>
       </c>
       <c r="T102" s="1">
-        <v>0</v>
+        <v>13345.12</v>
       </c>
       <c r="U102" s="1">
-        <v>93824</v>
+        <v>115999.9</v>
       </c>
       <c r="V102" t="s">
         <v>35</v>
@@ -8282,7 +8330,7 @@
         <v>1</v>
       </c>
       <c r="X102">
-        <v>93824</v>
+        <v>115999.9</v>
       </c>
     </row>
     <row r="103" spans="1:24">
@@ -8293,13 +8341,13 @@
         <v>24</v>
       </c>
       <c r="C103" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="D103" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E103" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="F103" t="s">
         <v>28</v>
@@ -8311,16 +8359,16 @@
         <v>30</v>
       </c>
       <c r="J103" t="s">
-        <v>368</v>
+        <v>252</v>
       </c>
       <c r="K103" t="s">
-        <v>369</v>
+        <v>253</v>
       </c>
       <c r="L103" t="s">
-        <v>370</v>
+        <v>254</v>
       </c>
       <c r="N103" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="O103" t="s">
         <v>34</v>
@@ -8332,13 +8380,13 @@
         <v>0</v>
       </c>
       <c r="S103" s="1">
-        <v>102654.78</v>
+        <v>345070.79645999998</v>
       </c>
       <c r="T103" s="1">
-        <v>13345.12</v>
+        <v>44859.203540000002</v>
       </c>
       <c r="U103" s="1">
-        <v>115999.9</v>
+        <v>389930</v>
       </c>
       <c r="V103" t="s">
         <v>35</v>
@@ -8347,7 +8395,7 @@
         <v>1</v>
       </c>
       <c r="X103">
-        <v>115999.9</v>
+        <v>389930</v>
       </c>
     </row>
     <row r="104" spans="1:24">
@@ -8376,16 +8424,16 @@
         <v>30</v>
       </c>
       <c r="J104" t="s">
-        <v>254</v>
+        <v>68</v>
       </c>
       <c r="K104" t="s">
-        <v>255</v>
+        <v>69</v>
       </c>
       <c r="L104" t="s">
-        <v>256</v>
+        <v>70</v>
       </c>
       <c r="N104" t="s">
-        <v>129</v>
+        <v>71</v>
       </c>
       <c r="O104" t="s">
         <v>34</v>
@@ -8397,13 +8445,13 @@
         <v>0</v>
       </c>
       <c r="S104" s="1">
-        <v>345070.79645999998</v>
+        <v>272160</v>
       </c>
       <c r="T104" s="1">
-        <v>44859.203540000002</v>
+        <v>35380.800000000003</v>
       </c>
       <c r="U104" s="1">
-        <v>389930</v>
+        <v>307540.8</v>
       </c>
       <c r="V104" t="s">
         <v>35</v>
@@ -8412,7 +8460,7 @@
         <v>1</v>
       </c>
       <c r="X104">
-        <v>389930</v>
+        <v>307540.8</v>
       </c>
     </row>
     <row r="105" spans="1:24">
@@ -8426,7 +8474,7 @@
         <v>373</v>
       </c>
       <c r="D105" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="E105" t="s">
         <v>374</v>
@@ -8441,16 +8489,16 @@
         <v>30</v>
       </c>
       <c r="J105" t="s">
-        <v>68</v>
+        <v>304</v>
       </c>
       <c r="K105" t="s">
-        <v>69</v>
+        <v>305</v>
       </c>
       <c r="L105" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="N105" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="O105" t="s">
         <v>34</v>
@@ -8462,13 +8510,13 @@
         <v>0</v>
       </c>
       <c r="S105" s="1">
-        <v>272160</v>
+        <v>1269.9114999999999</v>
       </c>
       <c r="T105" s="1">
-        <v>35380.800000000003</v>
+        <v>165.08850000000001</v>
       </c>
       <c r="U105" s="1">
-        <v>307540.8</v>
+        <v>1435</v>
       </c>
       <c r="V105" t="s">
         <v>35</v>
@@ -8477,7 +8525,7 @@
         <v>1</v>
       </c>
       <c r="X105">
-        <v>307540.8</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="106" spans="1:24">
@@ -8491,7 +8539,7 @@
         <v>375</v>
       </c>
       <c r="D106" t="s">
-        <v>77</v>
+        <v>242</v>
       </c>
       <c r="E106" t="s">
         <v>376</v>
@@ -8506,16 +8554,16 @@
         <v>30</v>
       </c>
       <c r="J106" t="s">
-        <v>306</v>
+        <v>31</v>
       </c>
       <c r="K106" t="s">
-        <v>307</v>
+        <v>32</v>
       </c>
       <c r="L106" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="N106" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="O106" t="s">
         <v>34</v>
@@ -8527,13 +8575,13 @@
         <v>0</v>
       </c>
       <c r="S106" s="1">
-        <v>1269.9114999999999</v>
+        <v>7000</v>
       </c>
       <c r="T106" s="1">
-        <v>165.08850000000001</v>
+        <v>0</v>
       </c>
       <c r="U106" s="1">
-        <v>1435</v>
+        <v>7000</v>
       </c>
       <c r="V106" t="s">
         <v>35</v>
@@ -8542,7 +8590,7 @@
         <v>1</v>
       </c>
       <c r="X106">
-        <v>1435</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="107" spans="1:24">
@@ -8556,7 +8604,7 @@
         <v>377</v>
       </c>
       <c r="D107" t="s">
-        <v>242</v>
+        <v>44</v>
       </c>
       <c r="E107" t="s">
         <v>378</v>
@@ -8571,16 +8619,16 @@
         <v>30</v>
       </c>
       <c r="J107" t="s">
-        <v>31</v>
+        <v>114</v>
       </c>
       <c r="K107" t="s">
-        <v>32</v>
+        <v>115</v>
       </c>
       <c r="L107" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="N107" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="O107" t="s">
         <v>34</v>
@@ -8592,13 +8640,13 @@
         <v>0</v>
       </c>
       <c r="S107" s="1">
-        <v>7000</v>
+        <v>5000</v>
       </c>
       <c r="T107" s="1">
         <v>0</v>
       </c>
       <c r="U107" s="1">
-        <v>7000</v>
+        <v>5000</v>
       </c>
       <c r="V107" t="s">
         <v>35</v>
@@ -8607,7 +8655,7 @@
         <v>1</v>
       </c>
       <c r="X107">
-        <v>7000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="108" spans="1:24">
@@ -8621,7 +8669,7 @@
         <v>379</v>
       </c>
       <c r="D108" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="E108" t="s">
         <v>380</v>
@@ -8636,16 +8684,16 @@
         <v>30</v>
       </c>
       <c r="J108" t="s">
-        <v>114</v>
+        <v>149</v>
       </c>
       <c r="K108" t="s">
-        <v>115</v>
+        <v>150</v>
       </c>
       <c r="L108" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="N108" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="O108" t="s">
         <v>34</v>
@@ -8657,13 +8705,13 @@
         <v>0</v>
       </c>
       <c r="S108" s="1">
-        <v>5000</v>
+        <v>58636.66</v>
       </c>
       <c r="T108" s="1">
-        <v>0</v>
+        <v>7622.77</v>
       </c>
       <c r="U108" s="1">
-        <v>5000</v>
+        <v>66259.429999999993</v>
       </c>
       <c r="V108" t="s">
         <v>35</v>
@@ -8672,7 +8720,7 @@
         <v>1</v>
       </c>
       <c r="X108">
-        <v>5000</v>
+        <v>66259.429999999993</v>
       </c>
     </row>
     <row r="109" spans="1:24">
@@ -8686,7 +8734,7 @@
         <v>381</v>
       </c>
       <c r="D109" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E109" t="s">
         <v>382</v>
@@ -8701,16 +8749,16 @@
         <v>30</v>
       </c>
       <c r="J109" t="s">
-        <v>149</v>
+        <v>336</v>
       </c>
       <c r="K109" t="s">
-        <v>150</v>
+        <v>337</v>
       </c>
       <c r="L109" t="s">
-        <v>64</v>
+        <v>282</v>
       </c>
       <c r="N109" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="O109" t="s">
         <v>34</v>
@@ -8722,13 +8770,13 @@
         <v>0</v>
       </c>
       <c r="S109" s="1">
-        <v>58636.66</v>
+        <v>32478</v>
       </c>
       <c r="T109" s="1">
-        <v>7622.77</v>
+        <v>4222.1400000000003</v>
       </c>
       <c r="U109" s="1">
-        <v>66259.429999999993</v>
+        <v>36700.14</v>
       </c>
       <c r="V109" t="s">
         <v>35</v>
@@ -8737,7 +8785,7 @@
         <v>1</v>
       </c>
       <c r="X109">
-        <v>66259.429999999993</v>
+        <v>36700.14</v>
       </c>
     </row>
     <row r="110" spans="1:24">
@@ -8751,7 +8799,7 @@
         <v>383</v>
       </c>
       <c r="D110" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E110" t="s">
         <v>384</v>
@@ -8766,16 +8814,16 @@
         <v>30</v>
       </c>
       <c r="J110" t="s">
-        <v>338</v>
+        <v>68</v>
       </c>
       <c r="K110" t="s">
-        <v>339</v>
+        <v>69</v>
       </c>
       <c r="L110" t="s">
-        <v>284</v>
+        <v>70</v>
       </c>
       <c r="N110" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="O110" t="s">
         <v>34</v>
@@ -8787,13 +8835,13 @@
         <v>0</v>
       </c>
       <c r="S110" s="1">
-        <v>32478</v>
+        <v>924464.48</v>
       </c>
       <c r="T110" s="1">
-        <v>4222.1400000000003</v>
+        <v>120180.38</v>
       </c>
       <c r="U110" s="1">
-        <v>36700.14</v>
+        <v>1044644.86</v>
       </c>
       <c r="V110" t="s">
         <v>35</v>
@@ -8802,7 +8850,7 @@
         <v>1</v>
       </c>
       <c r="X110">
-        <v>36700.14</v>
+        <v>1044644.86</v>
       </c>
     </row>
     <row r="111" spans="1:24">
@@ -8831,16 +8879,16 @@
         <v>30</v>
       </c>
       <c r="J111" t="s">
-        <v>68</v>
+        <v>387</v>
       </c>
       <c r="K111" t="s">
-        <v>69</v>
+        <v>388</v>
       </c>
       <c r="L111" t="s">
-        <v>70</v>
+        <v>389</v>
       </c>
       <c r="N111" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="O111" t="s">
         <v>34</v>
@@ -8852,13 +8900,13 @@
         <v>0</v>
       </c>
       <c r="S111" s="1">
-        <v>924464.48</v>
+        <v>30591.82</v>
       </c>
       <c r="T111" s="1">
-        <v>120180.38</v>
+        <v>3976.95</v>
       </c>
       <c r="U111" s="1">
-        <v>1044644.86</v>
+        <v>34568.769999999997</v>
       </c>
       <c r="V111" t="s">
         <v>35</v>
@@ -8867,7 +8915,7 @@
         <v>1</v>
       </c>
       <c r="X111">
-        <v>1044644.86</v>
+        <v>34568.769999999997</v>
       </c>
     </row>
     <row r="112" spans="1:24">
@@ -8878,13 +8926,13 @@
         <v>24</v>
       </c>
       <c r="C112" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="D112" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="E112" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="F112" t="s">
         <v>28</v>
@@ -8896,16 +8944,16 @@
         <v>30</v>
       </c>
       <c r="J112" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="K112" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="L112" t="s">
-        <v>391</v>
+        <v>217</v>
       </c>
       <c r="N112" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="O112" t="s">
         <v>34</v>
@@ -8917,13 +8965,13 @@
         <v>0</v>
       </c>
       <c r="S112" s="1">
-        <v>30591.82</v>
+        <v>20000</v>
       </c>
       <c r="T112" s="1">
-        <v>3976.95</v>
+        <v>2600</v>
       </c>
       <c r="U112" s="1">
-        <v>34568.769999999997</v>
+        <v>22600</v>
       </c>
       <c r="V112" t="s">
         <v>35</v>
@@ -8932,7 +8980,7 @@
         <v>1</v>
       </c>
       <c r="X112">
-        <v>34568.769999999997</v>
+        <v>22600</v>
       </c>
     </row>
     <row r="113" spans="1:24">
@@ -8943,13 +8991,13 @@
         <v>24</v>
       </c>
       <c r="C113" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="D113" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="E113" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="F113" t="s">
         <v>28</v>
@@ -8961,16 +9009,16 @@
         <v>30</v>
       </c>
       <c r="J113" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="K113" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="L113" t="s">
-        <v>217</v>
+        <v>389</v>
       </c>
       <c r="N113" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="O113" t="s">
         <v>34</v>
@@ -8982,13 +9030,13 @@
         <v>0</v>
       </c>
       <c r="S113" s="1">
-        <v>20000</v>
+        <v>59214.19</v>
       </c>
       <c r="T113" s="1">
-        <v>2600</v>
+        <v>7697.84</v>
       </c>
       <c r="U113" s="1">
-        <v>22600</v>
+        <v>66912.03</v>
       </c>
       <c r="V113" t="s">
         <v>35</v>
@@ -8997,7 +9045,7 @@
         <v>1</v>
       </c>
       <c r="X113">
-        <v>22600</v>
+        <v>66912.03</v>
       </c>
     </row>
     <row r="114" spans="1:24">
@@ -9011,7 +9059,7 @@
         <v>396</v>
       </c>
       <c r="D114" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="E114" t="s">
         <v>397</v>
@@ -9026,16 +9074,16 @@
         <v>30</v>
       </c>
       <c r="J114" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="K114" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
       <c r="L114" t="s">
-        <v>391</v>
+        <v>33</v>
       </c>
       <c r="N114" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="O114" t="s">
         <v>34</v>
@@ -9047,13 +9095,13 @@
         <v>0</v>
       </c>
       <c r="S114" s="1">
-        <v>59214.19</v>
+        <v>15575.23</v>
       </c>
       <c r="T114" s="1">
-        <v>7697.84</v>
+        <v>2024.78</v>
       </c>
       <c r="U114" s="1">
-        <v>66912.03</v>
+        <v>17600.009999999998</v>
       </c>
       <c r="V114" t="s">
         <v>35</v>
@@ -9062,7 +9110,7 @@
         <v>1</v>
       </c>
       <c r="X114">
-        <v>66912.03</v>
+        <v>17600.009999999998</v>
       </c>
     </row>
     <row r="115" spans="1:24">
@@ -9073,13 +9121,13 @@
         <v>24</v>
       </c>
       <c r="C115" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="D115" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="E115" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="F115" t="s">
         <v>28</v>
@@ -9091,16 +9139,16 @@
         <v>30</v>
       </c>
       <c r="J115" t="s">
-        <v>400</v>
+        <v>119</v>
       </c>
       <c r="K115" t="s">
-        <v>401</v>
+        <v>120</v>
       </c>
       <c r="L115" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="N115" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="O115" t="s">
         <v>34</v>
@@ -9112,13 +9160,13 @@
         <v>0</v>
       </c>
       <c r="S115" s="1">
-        <v>15575.23</v>
+        <v>10000</v>
       </c>
       <c r="T115" s="1">
-        <v>2024.78</v>
+        <v>0</v>
       </c>
       <c r="U115" s="1">
-        <v>17600.009999999998</v>
+        <v>10000</v>
       </c>
       <c r="V115" t="s">
         <v>35</v>
@@ -9127,7 +9175,7 @@
         <v>1</v>
       </c>
       <c r="X115">
-        <v>17600.009999999998</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="116" spans="1:24">
@@ -9135,16 +9183,16 @@
         <v>39015</v>
       </c>
       <c r="B116" t="s">
-        <v>24</v>
+        <v>402</v>
       </c>
       <c r="C116" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D116" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E116" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F116" t="s">
         <v>28</v>
@@ -9156,16 +9204,16 @@
         <v>30</v>
       </c>
       <c r="J116" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="K116" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
       <c r="L116" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="N116" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="O116" t="s">
         <v>34</v>
@@ -9177,13 +9225,13 @@
         <v>0</v>
       </c>
       <c r="S116" s="1">
-        <v>10000</v>
+        <v>2938</v>
       </c>
       <c r="T116" s="1">
         <v>0</v>
       </c>
       <c r="U116" s="1">
-        <v>10000</v>
+        <v>2938</v>
       </c>
       <c r="V116" t="s">
         <v>35</v>
@@ -9192,7 +9240,7 @@
         <v>1</v>
       </c>
       <c r="X116">
-        <v>10000</v>
+        <v>2938</v>
       </c>
     </row>
     <row r="117" spans="1:24">
@@ -9200,13 +9248,13 @@
         <v>39015</v>
       </c>
       <c r="B117" t="s">
-        <v>404</v>
+        <v>24</v>
       </c>
       <c r="C117" t="s">
         <v>405</v>
       </c>
       <c r="D117" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E117" t="s">
         <v>406</v>
@@ -9221,16 +9269,16 @@
         <v>30</v>
       </c>
       <c r="J117" t="s">
-        <v>88</v>
+        <v>366</v>
       </c>
       <c r="K117" t="s">
-        <v>89</v>
+        <v>367</v>
       </c>
       <c r="L117" t="s">
-        <v>90</v>
-      </c>
-      <c r="N117" t="s">
-        <v>94</v>
+        <v>368</v>
+      </c>
+      <c r="N117" s="3">
+        <v>401735</v>
       </c>
       <c r="O117" t="s">
         <v>34</v>
@@ -9242,13 +9290,13 @@
         <v>0</v>
       </c>
       <c r="S117" s="1">
-        <v>2938</v>
+        <v>79646.009999999995</v>
       </c>
       <c r="T117" s="1">
-        <v>0</v>
+        <v>10353.98</v>
       </c>
       <c r="U117" s="1">
-        <v>2938</v>
+        <v>89999.99</v>
       </c>
       <c r="V117" t="s">
         <v>35</v>
@@ -9257,7 +9305,7 @@
         <v>1</v>
       </c>
       <c r="X117">
-        <v>2938</v>
+        <v>89999.99</v>
       </c>
     </row>
     <row r="118" spans="1:24">
@@ -9271,10 +9319,10 @@
         <v>407</v>
       </c>
       <c r="D118" t="s">
-        <v>66</v>
+        <v>408</v>
       </c>
       <c r="E118" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="F118" t="s">
         <v>28</v>
@@ -9286,16 +9334,16 @@
         <v>30</v>
       </c>
       <c r="J118" t="s">
-        <v>368</v>
+        <v>410</v>
       </c>
       <c r="K118" t="s">
-        <v>369</v>
+        <v>411</v>
       </c>
       <c r="L118" t="s">
-        <v>370</v>
+        <v>64</v>
       </c>
       <c r="N118" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="O118" t="s">
         <v>34</v>
@@ -9307,13 +9355,13 @@
         <v>0</v>
       </c>
       <c r="S118" s="1">
-        <v>79646.009999999995</v>
+        <v>32690.26</v>
       </c>
       <c r="T118" s="1">
-        <v>10353.98</v>
+        <v>4249.74</v>
       </c>
       <c r="U118" s="1">
-        <v>89999.99</v>
+        <v>36940</v>
       </c>
       <c r="V118" t="s">
         <v>35</v>
@@ -9322,71 +9370,6 @@
         <v>1</v>
       </c>
       <c r="X118">
-        <v>89999.99</v>
-      </c>
-    </row>
-    <row r="119" spans="1:24">
-      <c r="A119">
-        <v>39015</v>
-      </c>
-      <c r="B119" t="s">
-        <v>24</v>
-      </c>
-      <c r="C119" t="s">
-        <v>409</v>
-      </c>
-      <c r="D119" t="s">
-        <v>410</v>
-      </c>
-      <c r="E119" t="s">
-        <v>411</v>
-      </c>
-      <c r="F119" t="s">
-        <v>28</v>
-      </c>
-      <c r="G119" t="s">
-        <v>29</v>
-      </c>
-      <c r="H119" t="s">
-        <v>30</v>
-      </c>
-      <c r="J119" t="s">
-        <v>412</v>
-      </c>
-      <c r="K119" t="s">
-        <v>413</v>
-      </c>
-      <c r="L119" t="s">
-        <v>64</v>
-      </c>
-      <c r="N119" t="s">
-        <v>71</v>
-      </c>
-      <c r="O119" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q119">
-        <v>0</v>
-      </c>
-      <c r="R119">
-        <v>0</v>
-      </c>
-      <c r="S119" s="1">
-        <v>32690.26</v>
-      </c>
-      <c r="T119" s="1">
-        <v>4249.74</v>
-      </c>
-      <c r="U119" s="1">
-        <v>36940</v>
-      </c>
-      <c r="V119" t="s">
-        <v>35</v>
-      </c>
-      <c r="W119">
-        <v>1</v>
-      </c>
-      <c r="X119">
         <v>36940</v>
       </c>
     </row>

</xml_diff>